<commit_message>
small fix and of y finance
</commit_message>
<xml_diff>
--- a/.xlsx/itd_time_percent.xlsx
+++ b/.xlsx/itd_time_percent.xlsx
@@ -451,447 +451,447 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45783.375</v>
+        <v>45785.375</v>
       </c>
       <c r="B2" t="n">
-        <v>0.002066991586672492</v>
+        <v>0.002000890919897798</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45783.37847222222</v>
+        <v>45785.37847222222</v>
       </c>
       <c r="B3" t="n">
-        <v>0.005306754522610258</v>
+        <v>0.005146220767290485</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45783.38194444445</v>
+        <v>45785.38194444445</v>
       </c>
       <c r="B4" t="n">
-        <v>0.007503348228124412</v>
+        <v>0.007309114207060435</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45783.38541666666</v>
+        <v>45785.38541666666</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05415506422664566</v>
+        <v>0.0528345396846035</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45783.38888888889</v>
+        <v>45785.38888888889</v>
       </c>
       <c r="B6" t="n">
-        <v>0.07830779018761022</v>
+        <v>0.07682729025092071</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45783.39236111111</v>
+        <v>45785.39236111111</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1068152401525096</v>
+        <v>0.105587160459568</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45783.39583333334</v>
+        <v>45785.39583333334</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1330970099770371</v>
+        <v>0.1320499672136994</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45783.39930555555</v>
+        <v>45785.39930555555</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1561225013899256</v>
+        <v>0.1550265514964979</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45783.40277777778</v>
+        <v>45785.40277777778</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1782000461066376</v>
+        <v>0.1769693118514202</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45783.40625</v>
+        <v>45785.40625</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2001334394176092</v>
+        <v>0.1989684840795836</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45783.40972222222</v>
+        <v>45785.40972222222</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2182416316268655</v>
+        <v>0.2171710197813316</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45783.41319444445</v>
+        <v>45785.41319444445</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2334780673375665</v>
+        <v>0.232682418585247</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45783.41666666666</v>
+        <v>45785.41666666666</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2449531431493842</v>
+        <v>0.2445766829652835</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45783.42013888889</v>
+        <v>45785.42013888889</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2606088543579794</v>
+        <v>0.2602061288480008</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45783.42361111111</v>
+        <v>45785.42361111111</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2734605137641954</v>
+        <v>0.2733402915799901</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45783.42708333334</v>
+        <v>45785.42708333334</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2897025789207949</v>
+        <v>0.2899181318025941</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45783.43055555555</v>
+        <v>45785.43055555555</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3054377130235121</v>
+        <v>0.3057263198382481</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45783.43402777778</v>
+        <v>45785.43402777778</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3212300103036891</v>
+        <v>0.3217240613408628</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45783.4375</v>
+        <v>45785.4375</v>
       </c>
       <c r="B20" t="n">
-        <v>0.336296221432862</v>
+        <v>0.3367974953216982</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45783.44097222222</v>
+        <v>45785.44097222222</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3504414318335003</v>
+        <v>0.3508931795126293</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45783.44444444445</v>
+        <v>45785.44444444445</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3651372301279986</v>
+        <v>0.3655014648706726</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45783.44791666666</v>
+        <v>45785.44791666666</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3795555275389423</v>
+        <v>0.3798428831291147</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45783.45138888889</v>
+        <v>45785.45138888889</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3927515733686595</v>
+        <v>0.3931052458931673</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45783.45486111111</v>
+        <v>45785.45486111111</v>
       </c>
       <c r="B25" t="n">
-        <v>0.406934561225083</v>
+        <v>0.4072928831411613</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45783.45833333334</v>
+        <v>45785.45833333334</v>
       </c>
       <c r="B26" t="n">
-        <v>0.4189432913786117</v>
+        <v>0.4193618208296876</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45783.46180555555</v>
+        <v>45785.46180555555</v>
       </c>
       <c r="B27" t="n">
-        <v>0.4316417277838495</v>
+        <v>0.4319521053632188</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45783.46527777778</v>
+        <v>45785.46527777778</v>
       </c>
       <c r="B28" t="n">
-        <v>0.4441100778059634</v>
+        <v>0.4443217043052283</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45783.46875</v>
+        <v>45785.46875</v>
       </c>
       <c r="B29" t="n">
-        <v>0.4557970944726276</v>
+        <v>0.4559775489999275</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45783.47222222222</v>
+        <v>45785.47222222222</v>
       </c>
       <c r="B30" t="n">
-        <v>0.4679992604262468</v>
+        <v>0.4681817390733403</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45783.47569444445</v>
+        <v>45785.47569444445</v>
       </c>
       <c r="B31" t="n">
-        <v>0.4816729597447818</v>
+        <v>0.4817875831033827</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45783.47916666666</v>
+        <v>45785.47916666666</v>
       </c>
       <c r="B32" t="n">
-        <v>0.4939284202991893</v>
+        <v>0.4939852457220174</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45783.54166666666</v>
+        <v>45785.54166666666</v>
       </c>
       <c r="B33" t="n">
-        <v>0.5083296024767094</v>
+        <v>0.5082356443978371</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45783.54513888889</v>
+        <v>45785.54513888889</v>
       </c>
       <c r="B34" t="n">
-        <v>0.5295523597688708</v>
+        <v>0.5293149471409798</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45783.54861111111</v>
+        <v>45785.54861111111</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5494027795348617</v>
+        <v>0.5491075733607118</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45783.55208333334</v>
+        <v>45785.55208333334</v>
       </c>
       <c r="B36" t="n">
-        <v>0.570931143115488</v>
+        <v>0.5706934972985998</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45783.55555555555</v>
+        <v>45785.55555555555</v>
       </c>
       <c r="B37" t="n">
-        <v>0.5937910649447129</v>
+        <v>0.5931401138147578</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45783.55902777778</v>
+        <v>45785.55902777778</v>
       </c>
       <c r="B38" t="n">
-        <v>0.6165627111480271</v>
+        <v>0.6157300390772882</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45783.5625</v>
+        <v>45785.5625</v>
       </c>
       <c r="B39" t="n">
-        <v>0.6387366960366822</v>
+        <v>0.6378314097499402</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45783.56597222222</v>
+        <v>45785.56597222222</v>
       </c>
       <c r="B40" t="n">
-        <v>0.661249716399368</v>
+        <v>0.6602726602467011</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45783.56944444445</v>
+        <v>45785.56944444445</v>
       </c>
       <c r="B41" t="n">
-        <v>0.6835906160647657</v>
+        <v>0.6827974516914428</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45783.57291666666</v>
+        <v>45785.57291666666</v>
       </c>
       <c r="B42" t="n">
-        <v>0.7069066462955342</v>
+        <v>0.7059592475232496</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45783.57638888889</v>
+        <v>45785.57638888889</v>
       </c>
       <c r="B43" t="n">
-        <v>0.727680465047675</v>
+        <v>0.7265784670215074</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45783.57986111111</v>
+        <v>45785.57986111111</v>
       </c>
       <c r="B44" t="n">
-        <v>0.7501943184942591</v>
+        <v>0.7490170380406582</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45783.58333333334</v>
+        <v>45785.58333333334</v>
       </c>
       <c r="B45" t="n">
-        <v>0.7720723889065308</v>
+        <v>0.7713136563251427</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45783.58680555555</v>
+        <v>45785.58680555555</v>
       </c>
       <c r="B46" t="n">
-        <v>0.7962162636041237</v>
+        <v>0.7961202444168476</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45783.59027777778</v>
+        <v>45785.59027777778</v>
       </c>
       <c r="B47" t="n">
-        <v>0.8202471330913723</v>
+        <v>0.8204249891797251</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45783.59375</v>
+        <v>45785.59375</v>
       </c>
       <c r="B48" t="n">
-        <v>0.845518238615772</v>
+        <v>0.8455421383400709</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45783.59722222222</v>
+        <v>45785.59722222222</v>
       </c>
       <c r="B49" t="n">
-        <v>0.8733924347640994</v>
+        <v>0.8733570072484979</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45783.60069444445</v>
+        <v>45785.60069444445</v>
       </c>
       <c r="B50" t="n">
-        <v>0.9034102844921829</v>
+        <v>0.9037553045706305</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45783.60416666666</v>
+        <v>45785.60416666666</v>
       </c>
       <c r="B51" t="n">
-        <v>0.934314192428088</v>
+        <v>0.9347689877083782</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45783.60763888889</v>
+        <v>45785.60763888889</v>
       </c>
       <c r="B52" t="n">
-        <v>0.9372631851391418</v>
+        <v>0.9377147464548174</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45783.61111111111</v>
+        <v>45785.61111111111</v>
       </c>
       <c r="B53" t="n">
-        <v>0.9395129106506767</v>
+        <v>0.9400047401639366</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45783.61458333334</v>
+        <v>45785.61458333334</v>
       </c>
       <c r="B54" t="n">
-        <v>0.9877369763197861</v>
+        <v>0.9882157395613993</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45783.61805555555</v>
+        <v>45785.61805555555</v>
       </c>
       <c r="B55" t="n">
-        <v>0.9928681908948165</v>
+        <v>0.9931331633185496</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45783.62152777778</v>
+        <v>45785.62152777778</v>
       </c>
       <c r="B56" t="n">
-        <v>0.9972338193612796</v>
+        <v>0.9973332952849573</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45783.625</v>
+        <v>45785.625</v>
       </c>
       <c r="B57" t="n">
         <v>1</v>

</xml_diff>